<commit_message>
updated overlay and spreadsheet.
</commit_message>
<xml_diff>
--- a/cms-ars-3.1-moderate-aws-rds-crunchy-data-postgresql-9-stig-overlay.xlsx
+++ b/cms-ars-3.1-moderate-aws-rds-crunchy-data-postgresql-9-stig-overlay.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhaynes/Documents/inspec/cms/cms-ars-3.1-moderate-aws-rds-crunchy-data-postgresql-9-stig-overlay/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{91B3282D-5352-BB4E-B70B-8D04F880C326}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{A5F26BEA-6D6A-D549-8390-243DFE9A3FF6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="0" windowWidth="33600" windowHeight="21000"/>
+    <workbookView xWindow="67200" yWindow="0" windowWidth="38400" windowHeight="21600"/>
   </bookViews>
   <sheets>
     <sheet name="cms-ars-3.1-moderate-aws-rds-cr" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="726" uniqueCount="510">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="807" uniqueCount="512">
   <si>
     <t>title</t>
   </si>
@@ -5481,6 +5481,12 @@
   To ensure that logging is enabled, review supplementary content APPENDIX-C for
   instructions on enabling logging.</t>
     </r>
+  </si>
+  <si>
+    <t>Does it differ from PostgresSQL STIG tailored for CMS ARS 3.1?</t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
 </sst>
 </file>
@@ -6359,10 +6365,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J81"/>
+  <dimension ref="A1:K81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J81" sqref="J81"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="29.6640625" defaultRowHeight="16"/>
@@ -6379,7 +6385,7 @@
     <col min="10" max="16384" width="29.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="17">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="34">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6410,8 +6416,11 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>510</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" ht="409.6">
+    <row r="2" spans="1:11" ht="409.6">
       <c r="A2" s="2" t="s">
         <v>487</v>
       </c>
@@ -6442,8 +6451,11 @@
       <c r="J2" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="K2" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" ht="409.6">
+    <row r="3" spans="1:11" ht="409.6">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -6474,8 +6486,11 @@
       <c r="J3" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="K3" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" ht="323">
+    <row r="4" spans="1:11" ht="323">
       <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
@@ -6506,8 +6521,11 @@
       <c r="J4" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="K4" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" ht="409.6">
+    <row r="5" spans="1:11" ht="409.6">
       <c r="A5" s="2" t="s">
         <v>31</v>
       </c>
@@ -6538,8 +6556,11 @@
       <c r="J5" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="K5" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" ht="409.6">
+    <row r="6" spans="1:11" ht="409.6">
       <c r="A6" s="2" t="s">
         <v>38</v>
       </c>
@@ -6570,8 +6591,11 @@
       <c r="J6" s="3" t="s">
         <v>40</v>
       </c>
+      <c r="K6" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" ht="409.6">
+    <row r="7" spans="1:11" ht="409.6">
       <c r="A7" s="2" t="s">
         <v>45</v>
       </c>
@@ -6602,8 +6626,11 @@
       <c r="J7" s="3" t="s">
         <v>47</v>
       </c>
+      <c r="K7" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="8" spans="1:10" ht="409.6">
+    <row r="8" spans="1:11" ht="409.6">
       <c r="A8" s="2" t="s">
         <v>52</v>
       </c>
@@ -6634,8 +6661,11 @@
       <c r="J8" s="3" t="s">
         <v>54</v>
       </c>
+      <c r="K8" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="9" spans="1:10" ht="372">
+    <row r="9" spans="1:11" ht="372">
       <c r="A9" s="2" t="s">
         <v>57</v>
       </c>
@@ -6666,8 +6696,11 @@
       <c r="J9" s="3" t="s">
         <v>59</v>
       </c>
+      <c r="K9" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="10" spans="1:10" ht="409.6">
+    <row r="10" spans="1:11" ht="409.6">
       <c r="A10" s="2" t="s">
         <v>61</v>
       </c>
@@ -6698,8 +6731,11 @@
       <c r="J10" s="3" t="s">
         <v>63</v>
       </c>
+      <c r="K10" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="11" spans="1:10" ht="409.6">
+    <row r="11" spans="1:11" ht="409.6">
       <c r="A11" s="4" t="s">
         <v>488</v>
       </c>
@@ -6730,8 +6766,11 @@
       <c r="J11" s="5" t="s">
         <v>68</v>
       </c>
+      <c r="K11" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="12" spans="1:10" ht="409.6">
+    <row r="12" spans="1:11" ht="409.6">
       <c r="A12" s="2" t="s">
         <v>72</v>
       </c>
@@ -6762,8 +6801,11 @@
       <c r="J12" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="K12" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="13" spans="1:10" ht="409.6">
+    <row r="13" spans="1:11" ht="409.6">
       <c r="A13" s="2" t="s">
         <v>79</v>
       </c>
@@ -6794,8 +6836,11 @@
       <c r="J13" s="5" t="s">
         <v>80</v>
       </c>
+      <c r="K13" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="14" spans="1:10" ht="409.6">
+    <row r="14" spans="1:11" ht="409.6">
       <c r="A14" s="2" t="s">
         <v>85</v>
       </c>
@@ -6826,8 +6871,11 @@
       <c r="J14" s="3" t="s">
         <v>87</v>
       </c>
+      <c r="K14" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="15" spans="1:10" ht="404">
+    <row r="15" spans="1:11" ht="404">
       <c r="A15" s="2" t="s">
         <v>90</v>
       </c>
@@ -6858,8 +6906,11 @@
       <c r="J15" s="3" t="s">
         <v>92</v>
       </c>
+      <c r="K15" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="16" spans="1:10" ht="409.6">
+    <row r="16" spans="1:11" ht="409.6">
       <c r="A16" s="4" t="s">
         <v>492</v>
       </c>
@@ -6890,8 +6941,11 @@
       <c r="J16" s="5" t="s">
         <v>97</v>
       </c>
+      <c r="K16" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="17" spans="1:10" ht="409.6">
+    <row r="17" spans="1:11" ht="409.6">
       <c r="A17" s="2" t="s">
         <v>100</v>
       </c>
@@ -6922,8 +6976,11 @@
       <c r="J17" s="3" t="s">
         <v>102</v>
       </c>
+      <c r="K17" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="18" spans="1:10" ht="409.6">
+    <row r="18" spans="1:11" ht="409.6">
       <c r="A18" s="2" t="s">
         <v>107</v>
       </c>
@@ -6954,8 +7011,11 @@
       <c r="J18" s="5" t="s">
         <v>108</v>
       </c>
+      <c r="K18" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="19" spans="1:10" ht="409.6">
+    <row r="19" spans="1:11" ht="409.6">
       <c r="A19" s="2" t="s">
         <v>113</v>
       </c>
@@ -6986,8 +7046,11 @@
       <c r="J19" s="3" t="s">
         <v>115</v>
       </c>
+      <c r="K19" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="20" spans="1:10" ht="204">
+    <row r="20" spans="1:11" ht="204">
       <c r="A20" s="2" t="s">
         <v>120</v>
       </c>
@@ -7018,8 +7081,11 @@
       <c r="J20" s="3" t="s">
         <v>123</v>
       </c>
+      <c r="K20" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="21" spans="1:10" ht="409.6">
+    <row r="21" spans="1:11" ht="409.6">
       <c r="A21" s="2" t="s">
         <v>128</v>
       </c>
@@ -7050,8 +7116,11 @@
       <c r="J21" s="3" t="s">
         <v>130</v>
       </c>
+      <c r="K21" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="22" spans="1:10" ht="409.6">
+    <row r="22" spans="1:11" ht="409.6">
       <c r="A22" s="2" t="s">
         <v>135</v>
       </c>
@@ -7082,8 +7151,11 @@
       <c r="J22" s="5" t="s">
         <v>136</v>
       </c>
+      <c r="K22" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="23" spans="1:10" ht="409.6">
+    <row r="23" spans="1:11" ht="409.6">
       <c r="A23" s="2" t="s">
         <v>140</v>
       </c>
@@ -7114,8 +7186,11 @@
       <c r="J23" s="3" t="s">
         <v>142</v>
       </c>
+      <c r="K23" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="24" spans="1:10" ht="409.6">
+    <row r="24" spans="1:11" ht="409.6">
       <c r="A24" s="2" t="s">
         <v>147</v>
       </c>
@@ -7146,8 +7221,11 @@
       <c r="J24" s="3" t="s">
         <v>149</v>
       </c>
+      <c r="K24" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="25" spans="1:10" ht="409.6">
+    <row r="25" spans="1:11" ht="409.6">
       <c r="A25" s="2" t="s">
         <v>154</v>
       </c>
@@ -7178,8 +7256,11 @@
       <c r="J25" s="3" t="s">
         <v>156</v>
       </c>
+      <c r="K25" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="26" spans="1:10" ht="409.6">
+    <row r="26" spans="1:11" ht="409.6">
       <c r="A26" s="2" t="s">
         <v>160</v>
       </c>
@@ -7210,8 +7291,11 @@
       <c r="J26" s="3" t="s">
         <v>162</v>
       </c>
+      <c r="K26" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="27" spans="1:10" ht="409.6">
+    <row r="27" spans="1:11" ht="409.6">
       <c r="A27" s="2" t="s">
         <v>167</v>
       </c>
@@ -7242,8 +7326,11 @@
       <c r="J27" s="3" t="s">
         <v>169</v>
       </c>
+      <c r="K27" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="28" spans="1:10" ht="409.6">
+    <row r="28" spans="1:11" ht="409.6">
       <c r="A28" s="2" t="s">
         <v>174</v>
       </c>
@@ -7274,8 +7361,11 @@
       <c r="J28" s="3" t="s">
         <v>176</v>
       </c>
+      <c r="K28" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="29" spans="1:10" ht="409.6">
+    <row r="29" spans="1:11" ht="409.6">
       <c r="A29" s="2" t="s">
         <v>181</v>
       </c>
@@ -7306,8 +7396,11 @@
       <c r="J29" s="3" t="s">
         <v>183</v>
       </c>
+      <c r="K29" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="30" spans="1:10" ht="409.6">
+    <row r="30" spans="1:11" ht="409.6">
       <c r="A30" s="2" t="s">
         <v>186</v>
       </c>
@@ -7338,8 +7431,11 @@
       <c r="J30" s="3" t="s">
         <v>188</v>
       </c>
+      <c r="K30" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="31" spans="1:10" ht="409.6">
+    <row r="31" spans="1:11" ht="409.6">
       <c r="A31" s="2" t="s">
         <v>193</v>
       </c>
@@ -7370,8 +7466,11 @@
       <c r="J31" s="3" t="s">
         <v>195</v>
       </c>
+      <c r="K31" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="32" spans="1:10" ht="409.6">
+    <row r="32" spans="1:11" ht="409.6">
       <c r="A32" s="2" t="s">
         <v>199</v>
       </c>
@@ -7402,8 +7501,11 @@
       <c r="J32" s="3" t="s">
         <v>201</v>
       </c>
+      <c r="K32" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="33" spans="1:10" ht="388">
+    <row r="33" spans="1:11" ht="388">
       <c r="A33" s="2" t="s">
         <v>206</v>
       </c>
@@ -7434,8 +7536,11 @@
       <c r="J33" s="3" t="s">
         <v>208</v>
       </c>
+      <c r="K33" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="34" spans="1:10" ht="372">
+    <row r="34" spans="1:11" ht="372">
       <c r="A34" s="2" t="s">
         <v>210</v>
       </c>
@@ -7466,8 +7571,11 @@
       <c r="J34" s="3" t="s">
         <v>212</v>
       </c>
+      <c r="K34" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="35" spans="1:10" ht="409.6">
+    <row r="35" spans="1:11" ht="409.6">
       <c r="A35" s="2" t="s">
         <v>215</v>
       </c>
@@ -7498,8 +7606,11 @@
       <c r="J35" s="5" t="s">
         <v>216</v>
       </c>
+      <c r="K35" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="36" spans="1:10" ht="409.6">
+    <row r="36" spans="1:11" ht="409.6">
       <c r="A36" s="2" t="s">
         <v>221</v>
       </c>
@@ -7530,8 +7641,11 @@
       <c r="J36" s="3" t="s">
         <v>223</v>
       </c>
+      <c r="K36" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="37" spans="1:10" ht="409.6">
+    <row r="37" spans="1:11" ht="409.6">
       <c r="A37" s="2" t="s">
         <v>228</v>
       </c>
@@ -7562,8 +7676,11 @@
       <c r="J37" s="3" t="s">
         <v>230</v>
       </c>
+      <c r="K37" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="38" spans="1:10" ht="409.6">
+    <row r="38" spans="1:11" ht="409.6">
       <c r="A38" s="2" t="s">
         <v>235</v>
       </c>
@@ -7594,8 +7711,11 @@
       <c r="J38" s="3" t="s">
         <v>237</v>
       </c>
+      <c r="K38" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="39" spans="1:10" ht="409.6">
+    <row r="39" spans="1:11" ht="409.6">
       <c r="A39" s="2" t="s">
         <v>242</v>
       </c>
@@ -7626,8 +7746,11 @@
       <c r="J39" s="5" t="s">
         <v>243</v>
       </c>
+      <c r="K39" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="40" spans="1:10" ht="388">
+    <row r="40" spans="1:11" ht="388">
       <c r="A40" s="2" t="s">
         <v>248</v>
       </c>
@@ -7658,8 +7781,11 @@
       <c r="J40" s="3" t="s">
         <v>249</v>
       </c>
+      <c r="K40" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="41" spans="1:10" ht="409.6">
+    <row r="41" spans="1:11" ht="409.6">
       <c r="A41" s="2" t="s">
         <v>252</v>
       </c>
@@ -7690,8 +7816,11 @@
       <c r="J41" s="3" t="s">
         <v>254</v>
       </c>
+      <c r="K41" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="42" spans="1:10" ht="409.6">
+    <row r="42" spans="1:11" ht="409.6">
       <c r="A42" s="2" t="s">
         <v>259</v>
       </c>
@@ -7722,8 +7851,11 @@
       <c r="J42" s="5" t="s">
         <v>260</v>
       </c>
+      <c r="K42" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="43" spans="1:10" ht="409.6">
+    <row r="43" spans="1:11" ht="409.6">
       <c r="A43" s="2" t="s">
         <v>265</v>
       </c>
@@ -7754,8 +7886,11 @@
       <c r="J43" s="3" t="s">
         <v>267</v>
       </c>
+      <c r="K43" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="44" spans="1:10" ht="409.6">
+    <row r="44" spans="1:11" ht="409.6">
       <c r="A44" s="2" t="s">
         <v>272</v>
       </c>
@@ -7786,8 +7921,11 @@
       <c r="J44" s="3" t="s">
         <v>274</v>
       </c>
+      <c r="K44" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="45" spans="1:10" ht="409.6">
+    <row r="45" spans="1:11" ht="409.6">
       <c r="A45" s="2" t="s">
         <v>279</v>
       </c>
@@ -7818,8 +7956,11 @@
       <c r="J45" s="3" t="s">
         <v>281</v>
       </c>
+      <c r="K45" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="46" spans="1:10" ht="409.6">
+    <row r="46" spans="1:11" ht="409.6">
       <c r="A46" s="2" t="s">
         <v>284</v>
       </c>
@@ -7850,8 +7991,11 @@
       <c r="J46" s="3" t="s">
         <v>286</v>
       </c>
+      <c r="K46" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="47" spans="1:10" ht="356">
+    <row r="47" spans="1:11" ht="356">
       <c r="A47" s="2" t="s">
         <v>291</v>
       </c>
@@ -7882,8 +8026,11 @@
       <c r="J47" s="3" t="s">
         <v>293</v>
       </c>
+      <c r="K47" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="48" spans="1:10" ht="409.6">
+    <row r="48" spans="1:11" ht="409.6">
       <c r="A48" s="2" t="s">
         <v>296</v>
       </c>
@@ -7914,8 +8061,11 @@
       <c r="J48" s="3" t="s">
         <v>297</v>
       </c>
+      <c r="K48" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="49" spans="1:10" ht="409.6">
+    <row r="49" spans="1:11" ht="409.6">
       <c r="A49" s="2" t="s">
         <v>300</v>
       </c>
@@ -7946,8 +8096,11 @@
       <c r="J49" s="3" t="s">
         <v>302</v>
       </c>
+      <c r="K49" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="50" spans="1:10" ht="372">
+    <row r="50" spans="1:11" ht="372">
       <c r="A50" s="2" t="s">
         <v>307</v>
       </c>
@@ -7978,8 +8131,11 @@
       <c r="J50" s="3" t="s">
         <v>308</v>
       </c>
+      <c r="K50" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="51" spans="1:10" ht="409.6">
+    <row r="51" spans="1:11" ht="409.6">
       <c r="A51" s="2" t="s">
         <v>311</v>
       </c>
@@ -8010,8 +8166,11 @@
       <c r="J51" s="3" t="s">
         <v>313</v>
       </c>
+      <c r="K51" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="52" spans="1:10" ht="409.6">
+    <row r="52" spans="1:11" ht="409.6">
       <c r="A52" s="4" t="s">
         <v>502</v>
       </c>
@@ -8042,8 +8201,11 @@
       <c r="J52" s="5" t="s">
         <v>317</v>
       </c>
+      <c r="K52" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="53" spans="1:10" ht="409.6">
+    <row r="53" spans="1:11" ht="409.6">
       <c r="A53" s="2" t="s">
         <v>320</v>
       </c>
@@ -8074,8 +8236,11 @@
       <c r="J53" s="3" t="s">
         <v>322</v>
       </c>
+      <c r="K53" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="54" spans="1:10" ht="409.6">
+    <row r="54" spans="1:11" ht="409.6">
       <c r="A54" s="2" t="s">
         <v>327</v>
       </c>
@@ -8106,8 +8271,11 @@
       <c r="J54" s="3" t="s">
         <v>329</v>
       </c>
+      <c r="K54" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="55" spans="1:10" ht="409.6">
+    <row r="55" spans="1:11" ht="409.6">
       <c r="A55" s="2" t="s">
         <v>334</v>
       </c>
@@ -8138,8 +8306,11 @@
       <c r="J55" s="3" t="s">
         <v>336</v>
       </c>
+      <c r="K55" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="56" spans="1:10" ht="388">
+    <row r="56" spans="1:11" ht="388">
       <c r="A56" s="2" t="s">
         <v>339</v>
       </c>
@@ -8170,8 +8341,11 @@
       <c r="J56" s="3" t="s">
         <v>341</v>
       </c>
+      <c r="K56" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="57" spans="1:10" ht="356">
+    <row r="57" spans="1:11" ht="356">
       <c r="A57" s="2" t="s">
         <v>344</v>
       </c>
@@ -8202,8 +8376,11 @@
       <c r="J57" s="3" t="s">
         <v>346</v>
       </c>
+      <c r="K57" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="58" spans="1:10" ht="409.6">
+    <row r="58" spans="1:11" ht="409.6">
       <c r="A58" s="2" t="s">
         <v>351</v>
       </c>
@@ -8234,8 +8411,11 @@
       <c r="J58" s="3" t="s">
         <v>353</v>
       </c>
+      <c r="K58" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="59" spans="1:10" ht="409.6">
+    <row r="59" spans="1:11" ht="409.6">
       <c r="A59" s="2" t="s">
         <v>358</v>
       </c>
@@ -8266,8 +8446,11 @@
       <c r="J59" s="3" t="s">
         <v>359</v>
       </c>
+      <c r="K59" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="60" spans="1:10" ht="409.6">
+    <row r="60" spans="1:11" ht="409.6">
       <c r="A60" s="2" t="s">
         <v>363</v>
       </c>
@@ -8298,8 +8481,11 @@
       <c r="J60" s="3" t="s">
         <v>365</v>
       </c>
+      <c r="K60" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="61" spans="1:10" ht="409.6">
+    <row r="61" spans="1:11" ht="409.6">
       <c r="A61" s="2" t="s">
         <v>369</v>
       </c>
@@ -8330,8 +8516,11 @@
       <c r="J61" s="5" t="s">
         <v>370</v>
       </c>
+      <c r="K61" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="62" spans="1:10" ht="372">
+    <row r="62" spans="1:11" ht="372">
       <c r="A62" s="2" t="s">
         <v>375</v>
       </c>
@@ -8362,8 +8551,11 @@
       <c r="J62" s="3" t="s">
         <v>377</v>
       </c>
+      <c r="K62" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="63" spans="1:10" ht="409.6">
+    <row r="63" spans="1:11" ht="409.6">
       <c r="A63" s="2" t="s">
         <v>380</v>
       </c>
@@ -8394,8 +8586,11 @@
       <c r="J63" s="3" t="s">
         <v>382</v>
       </c>
+      <c r="K63" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="64" spans="1:10" ht="409.6">
+    <row r="64" spans="1:11" ht="409.6">
       <c r="A64" s="2" t="s">
         <v>385</v>
       </c>
@@ -8426,8 +8621,11 @@
       <c r="J64" s="3" t="s">
         <v>387</v>
       </c>
+      <c r="K64" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="65" spans="1:10" ht="409.6">
+    <row r="65" spans="1:11" ht="409.6">
       <c r="A65" s="2" t="s">
         <v>392</v>
       </c>
@@ -8458,8 +8656,11 @@
       <c r="J65" s="3" t="s">
         <v>394</v>
       </c>
+      <c r="K65" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="66" spans="1:10" ht="409.6">
+    <row r="66" spans="1:11" ht="409.6">
       <c r="A66" s="2" t="s">
         <v>397</v>
       </c>
@@ -8490,8 +8691,11 @@
       <c r="J66" s="3" t="s">
         <v>399</v>
       </c>
+      <c r="K66" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="67" spans="1:10" ht="409.6">
+    <row r="67" spans="1:11" ht="409.6">
       <c r="A67" s="2" t="s">
         <v>402</v>
       </c>
@@ -8510,8 +8714,11 @@
       <c r="J67" s="3" t="s">
         <v>406</v>
       </c>
+      <c r="K67" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="68" spans="1:10" ht="409.6">
+    <row r="68" spans="1:11" ht="409.6">
       <c r="A68" s="2" t="s">
         <v>407</v>
       </c>
@@ -8542,8 +8749,11 @@
       <c r="J68" s="3" t="s">
         <v>409</v>
       </c>
+      <c r="K68" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="69" spans="1:10" ht="409.6">
+    <row r="69" spans="1:11" ht="409.6">
       <c r="A69" s="2" t="s">
         <v>412</v>
       </c>
@@ -8574,8 +8784,11 @@
       <c r="J69" s="3" t="s">
         <v>414</v>
       </c>
+      <c r="K69" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="70" spans="1:10" ht="409.6">
+    <row r="70" spans="1:11" ht="409.6">
       <c r="A70" s="2" t="s">
         <v>419</v>
       </c>
@@ -8606,8 +8819,11 @@
       <c r="J70" s="3" t="s">
         <v>421</v>
       </c>
+      <c r="K70" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="71" spans="1:10" ht="409.6">
+    <row r="71" spans="1:11" ht="409.6">
       <c r="A71" s="2" t="s">
         <v>426</v>
       </c>
@@ -8638,8 +8854,11 @@
       <c r="J71" s="3" t="s">
         <v>428</v>
       </c>
+      <c r="K71" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="72" spans="1:10" ht="409.6">
+    <row r="72" spans="1:11" ht="409.6">
       <c r="A72" s="2" t="s">
         <v>431</v>
       </c>
@@ -8670,8 +8889,11 @@
       <c r="J72" s="3" t="s">
         <v>433</v>
       </c>
+      <c r="K72" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="73" spans="1:10" ht="409.6">
+    <row r="73" spans="1:11" ht="409.6">
       <c r="A73" s="2" t="s">
         <v>435</v>
       </c>
@@ -8702,8 +8924,11 @@
       <c r="J73" s="3" t="s">
         <v>437</v>
       </c>
+      <c r="K73" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="74" spans="1:10" ht="409.6">
+    <row r="74" spans="1:11" ht="409.6">
       <c r="A74" s="2" t="s">
         <v>438</v>
       </c>
@@ -8734,8 +8959,11 @@
       <c r="J74" s="3" t="s">
         <v>440</v>
       </c>
+      <c r="K74" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="75" spans="1:10" ht="409.6">
+    <row r="75" spans="1:11" ht="409.6">
       <c r="A75" s="2" t="s">
         <v>445</v>
       </c>
@@ -8766,8 +8994,11 @@
       <c r="J75" s="3" t="s">
         <v>447</v>
       </c>
+      <c r="K75" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="76" spans="1:10" ht="388">
+    <row r="76" spans="1:11" ht="388">
       <c r="A76" s="2" t="s">
         <v>452</v>
       </c>
@@ -8798,8 +9029,11 @@
       <c r="J76" s="3" t="s">
         <v>454</v>
       </c>
+      <c r="K76" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="77" spans="1:10" ht="409.6">
+    <row r="77" spans="1:11" ht="409.6">
       <c r="A77" s="2" t="s">
         <v>459</v>
       </c>
@@ -8830,8 +9064,11 @@
       <c r="J77" s="3" t="s">
         <v>461</v>
       </c>
+      <c r="K77" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="78" spans="1:10" ht="409.6">
+    <row r="78" spans="1:11" ht="409.6">
       <c r="A78" s="2" t="s">
         <v>464</v>
       </c>
@@ -8862,8 +9099,11 @@
       <c r="J78" s="3" t="s">
         <v>466</v>
       </c>
+      <c r="K78" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="79" spans="1:10" ht="409.6">
+    <row r="79" spans="1:11" ht="409.6">
       <c r="A79" s="2" t="s">
         <v>470</v>
       </c>
@@ -8894,8 +9134,11 @@
       <c r="J79" s="3" t="s">
         <v>472</v>
       </c>
+      <c r="K79" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="80" spans="1:10" ht="409.6">
+    <row r="80" spans="1:11" ht="409.6">
       <c r="A80" s="4" t="s">
         <v>507</v>
       </c>
@@ -8926,8 +9169,11 @@
       <c r="J80" s="5" t="s">
         <v>477</v>
       </c>
+      <c r="K80" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
-    <row r="81" spans="1:10" ht="409.6">
+    <row r="81" spans="1:11" ht="409.6">
       <c r="A81" s="2" t="s">
         <v>481</v>
       </c>
@@ -8957,6 +9203,9 @@
       </c>
       <c r="J81" s="3" t="s">
         <v>483</v>
+      </c>
+      <c r="K81" s="2" t="s">
+        <v>511</v>
       </c>
     </row>
   </sheetData>

</xml_diff>